<commit_message>
Pushing excel sheets for create Material Scenarios
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Material_Data.xlsx
+++ b/Mendix/input/data/Global_Material_Data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SatishKumarSundaramo\git\Mendix_New\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\New folder\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E1194-F6E5-4D25-8B96-8C98E8BF64BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{92753D1E-95E7-49CB-AD96-B588CC3DB29F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="YROH" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,10 +407,6 @@
     <t>Costing Method - Sales</t>
   </si>
   <si>
-    <t xml:space="preserve"> 
-Malt Pale C6 DE Koblenz </t>
-  </si>
-  <si>
     <t xml:space="preserve">
 CMG0006
 </t>
@@ -472,12 +467,15 @@
   </si>
   <si>
     <t>SG001OC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malt Pale C6 DE Koblenz Automation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -572,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -597,6 +595,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,95 +911,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1D1E45-5652-489D-98CC-1DC9815FE9A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="9.140625" style="8"/>
-    <col min="40" max="40" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="41" max="45" width="9.140625" style="8"/>
-    <col min="46" max="46" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="9.109375" style="8"/>
+    <col min="40" max="40" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="41" max="45" width="9.109375" style="8"/>
+    <col min="46" max="46" width="20.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="31.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="21.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="31.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="21.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="20.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="31.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="20.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="31.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="22.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="26" style="6" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="27.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="26.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="23.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="20.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="24.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="27.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="26.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="23.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="21" style="6" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="31.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="82" max="16384" width="9.140625" style="6"/>
+    <col min="80" max="80" width="11.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="31.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="82" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:81" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>89</v>
       </c>
@@ -1366,7 +1367,7 @@
       <c r="AV2" s="7"/>
       <c r="AW2" s="7"/>
     </row>
-    <row r="3" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>89</v>
       </c>
@@ -1491,7 +1492,7 @@
       <c r="AV3" s="7"/>
       <c r="AW3" s="7"/>
     </row>
-    <row r="4" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>90</v>
       </c>
@@ -1638,9 +1639,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>94</v>
@@ -1651,20 +1652,20 @@
       <c r="D5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>127</v>
+      <c r="E5" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="F5" s="4">
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -1673,7 +1674,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>41</v>
@@ -1694,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T5" s="10" t="s">
         <v>46</v>
@@ -1703,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W5" s="10" t="s">
         <v>64</v>
@@ -1730,7 +1731,7 @@
         <v>49</v>
       </c>
       <c r="AE5" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>64</v>
@@ -1751,10 +1752,10 @@
         <v>52</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AN5" s="7" t="s">
         <v>64</v>
@@ -1799,13 +1800,13 @@
         <v>1</v>
       </c>
       <c r="BB5" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BC5" s="6">
         <v>4</v>
       </c>
       <c r="BD5" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BE5" s="12" t="s">
         <v>39</v>
@@ -1814,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="BG5" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BH5" s="13">
         <v>0</v>
@@ -1832,19 +1833,19 @@
         <v>51</v>
       </c>
       <c r="BM5" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BN5" s="13" t="s">
         <v>51</v>
       </c>
       <c r="BO5" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="BP5" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="BP5" s="13" t="s">
+      <c r="BQ5" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="BQ5" s="13" t="s">
-        <v>140</v>
       </c>
       <c r="BR5" s="13">
         <v>7</v>
@@ -1865,20 +1866,20 @@
         <v>7</v>
       </c>
       <c r="BX5" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="BY5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BZ5" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="BY5" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="BZ5" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="CA5" s="13"/>
       <c r="CB5" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="CC5" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing only global material excel
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Material_Data.xlsx
+++ b/Mendix/input/data/Global_Material_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\New folder\MIP\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD53275-99C1-4BB4-BAD1-30074507D281}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YROH" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="150">
   <si>
     <t>Fields</t>
   </si>
@@ -470,12 +471,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Malt Pale C6 DE Koblenz Automation</t>
+  </si>
+  <si>
+    <t>BE01</t>
+  </si>
+  <si>
+    <t>Create_Material_with_Questionnaire_only_Global_SAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -911,17 +918,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="7.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.5546875" style="6" bestFit="1" customWidth="1"/>
@@ -1647,7 +1654,7 @@
         <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>76</v>
@@ -1880,6 +1887,119 @@
       </c>
       <c r="CC5" s="13" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:81" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK6" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing improvements and latest methods to add Bank Data to vendorNAV
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Material_Data.xlsx
+++ b/Mendix/input/data/Global_Material_Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\MIP\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\New folder\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD53275-99C1-4BB4-BAD1-30074507D281}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="YROH" sheetId="1" r:id="rId1"/>
@@ -482,7 +481,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -918,11 +917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1921,7 +1920,7 @@
         <v>38</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>40</v>
@@ -1930,7 +1929,7 @@
         <v>41</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>38</v>
@@ -1956,17 +1955,17 @@
       <c r="V6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="W6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="X6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z6" s="10" t="s">
-        <v>42</v>
+      <c r="W6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AA6" s="10" t="s">
         <v>47</v>
@@ -1980,14 +1979,14 @@
       <c r="AD6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="AE6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG6" s="10" t="s">
-        <v>42</v>
+      <c r="AE6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AH6" s="10" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Change Material Global only SAP
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Material_Data.xlsx
+++ b/Mendix/input/data/Global_Material_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\MIP\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Avaniheineken\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD53275-99C1-4BB4-BAD1-30074507D281}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C767657-3E4D-4E80-92EC-DEE057EFB99E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="153">
   <si>
     <t>Fields</t>
   </si>
@@ -477,6 +477,15 @@
   </si>
   <si>
     <t>Create_Material_with_Questionnaire_only_Global_SAP</t>
+  </si>
+  <si>
+    <t>3.Change_Material_global_only</t>
+  </si>
+  <si>
+    <t>Changing Material Descript</t>
+  </si>
+  <si>
+    <t>CMG0012</t>
   </si>
 </sst>
 </file>
@@ -919,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC6"/>
+  <dimension ref="A1:CC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1897,7 +1906,7 @@
         <v>149</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>76</v>
@@ -1999,6 +2008,119 @@
         <v>50</v>
       </c>
       <c r="AK6" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:81" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK7" s="10" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committing stabilized code for change material Nav as per current flow
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Material_Data.xlsx
+++ b/Mendix/input/data/Global_Material_Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Avaniheineken\MIP\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\MIP\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2D57C1-79CF-4FED-9196-80F3BBE3B1EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" tabRatio="603"/>
   </bookViews>
   <sheets>
     <sheet name="YROH" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="151">
   <si>
     <t>Fields</t>
   </si>
@@ -301,9 +300,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Test Create 1</t>
   </si>
   <si>
     <t>02, Keg</t>
@@ -480,12 +476,15 @@
   </si>
   <si>
     <t>3.Change_Material_global_only</t>
+  </si>
+  <si>
+    <t>Test Create Automation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -921,11 +920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,100 +1155,100 @@
         <v>87</v>
       </c>
       <c r="AX1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AY1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="BA1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BB1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BC1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="BC1" s="9" t="s">
+      <c r="BD1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BD1" s="9" t="s">
+      <c r="BE1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="BE1" s="9" t="s">
+      <c r="BF1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="BF1" s="9" t="s">
+      <c r="BG1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BG1" s="9" t="s">
+      <c r="BH1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BH1" s="9" t="s">
+      <c r="BI1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BI1" s="9" t="s">
+      <c r="BJ1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="BJ1" s="9" t="s">
+      <c r="BK1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="BK1" s="9" t="s">
+      <c r="BL1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="BM1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="BM1" s="9" t="s">
+      <c r="BN1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="BN1" s="9" t="s">
+      <c r="BO1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="BO1" s="9" t="s">
+      <c r="BP1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="BP1" s="9" t="s">
+      <c r="BQ1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="BQ1" s="9" t="s">
+      <c r="BR1" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="BR1" s="9" t="s">
+      <c r="BS1" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="BS1" s="9" t="s">
+      <c r="BT1" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="BT1" s="9" t="s">
+      <c r="BU1" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="BU1" s="9" t="s">
+      <c r="BV1" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="BV1" s="9" t="s">
+      <c r="BW1" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="BW1" s="9" t="s">
+      <c r="BX1" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="BX1" s="9" t="s">
+      <c r="BY1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="BY1" s="9" t="s">
+      <c r="BZ1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="BZ1" s="9" t="s">
+      <c r="CA1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="CA1" s="9" t="s">
+      <c r="CB1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="CB1" s="9" t="s">
+      <c r="CC1" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="CC1" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1510,19 +1509,19 @@
         <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>44</v>
@@ -1534,14 +1533,16 @@
         <v>77</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="M4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>77</v>
@@ -1568,16 +1569,16 @@
         <v>67</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>47</v>
@@ -1592,13 +1593,13 @@
         <v>49</v>
       </c>
       <c r="AE4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="AF4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="AG4" s="10" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="AH4" s="10" t="s">
         <v>50</v>
@@ -1619,10 +1620,10 @@
         <v>68</v>
       </c>
       <c r="AN4" s="7" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="AO4" s="7" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="AP4" s="7" t="s">
         <v>69</v>
@@ -1640,7 +1641,7 @@
         <v>73</v>
       </c>
       <c r="AU4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AV4" s="7" t="s">
         <v>74</v>
@@ -1651,31 +1652,31 @@
     </row>
     <row r="5" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>76</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F5" s="4">
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -1684,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>41</v>
@@ -1705,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T5" s="10" t="s">
         <v>46</v>
@@ -1714,7 +1715,7 @@
         <v>1</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W5" s="10" t="s">
         <v>64</v>
@@ -1741,7 +1742,7 @@
         <v>49</v>
       </c>
       <c r="AE5" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>64</v>
@@ -1762,10 +1763,10 @@
         <v>52</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AN5" s="7" t="s">
         <v>64</v>
@@ -1789,7 +1790,7 @@
         <v>73</v>
       </c>
       <c r="AU5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AV5" s="7" t="s">
         <v>74</v>
@@ -1810,13 +1811,13 @@
         <v>1</v>
       </c>
       <c r="BB5" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BC5" s="6">
         <v>4</v>
       </c>
       <c r="BD5" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BE5" s="12" t="s">
         <v>39</v>
@@ -1825,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="BG5" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BH5" s="13">
         <v>0</v>
@@ -1843,19 +1844,19 @@
         <v>51</v>
       </c>
       <c r="BM5" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BN5" s="13" t="s">
         <v>51</v>
       </c>
       <c r="BO5" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP5" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="BP5" s="13" t="s">
+      <c r="BQ5" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="BQ5" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="BR5" s="13">
         <v>7</v>
@@ -1876,28 +1877,28 @@
         <v>7</v>
       </c>
       <c r="BX5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BY5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="BZ5" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="BY5" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="BZ5" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="CA5" s="13"/>
       <c r="CB5" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="CC5" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>91</v>
@@ -2007,10 +2008,10 @@
     </row>
     <row r="7" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>91</v>

</xml_diff>